<commit_message>
zoom level = 15 update
</commit_message>
<xml_diff>
--- a/newsatel.xlsx
+++ b/newsatel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcao1\PycharmProjects\aiProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D375558-79E2-4A7C-8266-A42AABB2D6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2163A6-76CD-4A24-B7B7-A4506F1B9C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="5040" windowWidth="13200" windowHeight="9113" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="12563" windowHeight="5813" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B50"/>
+    <sheetView tabSelected="1" topLeftCell="A296" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -461,338 +461,2314 @@
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
-        <v>26.212399999999999</v>
+        <v>26.120899999999999</v>
       </c>
       <c r="B9" s="2">
-        <v>-81.840100000000007</v>
+        <v>-80.127899999999997</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
-        <v>26.120899999999999</v>
+        <v>28.612200000000001</v>
       </c>
       <c r="B10" s="2">
-        <v>-80.127899999999997</v>
+        <v>-81.200900000000004</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
-        <v>28.612200000000001</v>
+        <v>27.336400000000001</v>
       </c>
       <c r="B11" s="2">
-        <v>-81.200900000000004</v>
+        <v>-82.530699999999996</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
-        <v>27.336400000000001</v>
+        <v>29.187200000000001</v>
       </c>
       <c r="B12" s="2">
-        <v>-82.530699999999996</v>
+        <v>-82.140100000000004</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
-        <v>29.187200000000001</v>
+        <v>29.619700000000002</v>
       </c>
       <c r="B13" s="2">
-        <v>-82.140100000000004</v>
+        <v>-82.383200000000002</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
-        <v>29.619700000000002</v>
+        <v>30.421299999999999</v>
       </c>
       <c r="B14" s="2">
-        <v>-82.383200000000002</v>
+        <v>-87.216899999999995</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
-        <v>30.421299999999999</v>
+        <v>28.1189</v>
       </c>
       <c r="B15" s="2">
-        <v>-87.216899999999995</v>
+        <v>-80.633700000000005</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
-        <v>28.1189</v>
+        <v>30.421299999999999</v>
       </c>
       <c r="B16" s="2">
-        <v>-80.633700000000005</v>
+        <v>-86.617000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
-        <v>30.421299999999999</v>
+        <v>25.788900000000002</v>
       </c>
       <c r="B17" s="2">
-        <v>-86.617000000000004</v>
+        <v>-80.226399999999998</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
-        <v>25.788900000000002</v>
+        <v>28.692799999999998</v>
       </c>
       <c r="B18" s="2">
-        <v>-80.226399999999998</v>
+        <v>-81.3506</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
-        <v>28.692799999999998</v>
+        <v>26.640599999999999</v>
       </c>
       <c r="B19" s="2">
-        <v>-81.3506</v>
+        <v>-81.872299999999996</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
-        <v>28.1</v>
+        <v>30.200600000000001</v>
       </c>
       <c r="B20" s="2">
-        <v>-81.601799999999997</v>
+        <v>-81.6173</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
-        <v>29.206800000000001</v>
+        <v>28.034500000000001</v>
       </c>
       <c r="B21" s="2">
-        <v>-81.009399999999999</v>
+        <v>-80.588700000000003</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
-        <v>26.640599999999999</v>
+        <v>27.3413</v>
       </c>
       <c r="B22" s="2">
-        <v>-81.872299999999996</v>
+        <v>-82.528599999999997</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
-        <v>30.027200000000001</v>
+        <v>28.5383</v>
       </c>
       <c r="B23" s="2">
-        <v>-81.732900000000001</v>
+        <v>-81.379199999999997</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
-        <v>30.200600000000001</v>
+        <v>30.458300000000001</v>
       </c>
       <c r="B24" s="2">
-        <v>-81.6173</v>
+        <v>-84.280699999999996</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
-        <v>28.034500000000001</v>
+        <v>26.0505</v>
       </c>
       <c r="B25" s="2">
-        <v>-80.588700000000003</v>
+        <v>-80.136399999999995</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
-        <v>27.3413</v>
+        <v>27.767600000000002</v>
       </c>
       <c r="B26" s="2">
-        <v>-82.528599999999997</v>
+        <v>-82.640299999999996</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A27" s="2">
-        <v>28.5383</v>
+        <v>27.994199999999999</v>
       </c>
       <c r="B27" s="2">
-        <v>-81.379199999999997</v>
+        <v>-82.445099999999996</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
-        <v>26.6477</v>
+        <v>27.926300000000001</v>
       </c>
       <c r="B28" s="2">
-        <v>-81.872299999999996</v>
+        <v>-82.793000000000006</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" s="2">
-        <v>28.223800000000001</v>
+        <v>28.0809</v>
       </c>
       <c r="B29" s="2">
-        <v>-81.648799999999994</v>
+        <v>-80.608099999999993</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
-        <v>30.458300000000001</v>
+        <v>27.913599999999999</v>
       </c>
       <c r="B30" s="2">
-        <v>-84.280699999999996</v>
+        <v>-82.320999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
-        <v>26.0505</v>
+        <v>28.558900000000001</v>
       </c>
       <c r="B31" s="2">
-        <v>-80.136399999999995</v>
+        <v>-81.415400000000005</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" s="2">
-        <v>28.0685</v>
+        <v>28.818200000000001</v>
       </c>
       <c r="B32" s="2">
-        <v>-82.759299999999996</v>
+        <v>-81.734700000000004</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
-        <v>27.767600000000002</v>
+        <v>29.495799999999999</v>
       </c>
       <c r="B33" s="2">
-        <v>-82.640299999999996</v>
+        <v>-81.670599999999993</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A34" s="2">
-        <v>27.994199999999999</v>
+        <v>26.154199999999999</v>
       </c>
       <c r="B34" s="2">
-        <v>-82.445099999999996</v>
+        <v>-80.299800000000005</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A35" s="2">
-        <v>27.926300000000001</v>
+        <v>29.728999999999999</v>
       </c>
       <c r="B35" s="2">
-        <v>-82.793000000000006</v>
+        <v>-85.032200000000003</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A36" s="2">
-        <v>28.0809</v>
+        <v>30.080200000000001</v>
       </c>
       <c r="B36" s="2">
-        <v>-80.608099999999993</v>
+        <v>-81.709299999999999</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
-        <v>27.092199999999998</v>
+        <v>29.884899999999998</v>
       </c>
       <c r="B37" s="2">
-        <v>-82.509799999999998</v>
+        <v>-81.3155</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A38" s="2">
-        <v>27.913599999999999</v>
+        <v>27.9726</v>
       </c>
       <c r="B38" s="2">
-        <v>-82.320999999999998</v>
+        <v>-82.467600000000004</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
-        <v>28.558900000000001</v>
+        <v>28.121600000000001</v>
       </c>
       <c r="B39" s="2">
-        <v>-81.415400000000005</v>
+        <v>-81.625</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A40" s="2">
-        <v>28.818200000000001</v>
+        <v>26.1386</v>
       </c>
       <c r="B40" s="2">
-        <v>-81.734700000000004</v>
+        <v>-80.2209</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" s="2">
-        <v>29.495799999999999</v>
+        <v>28.047999999999998</v>
       </c>
       <c r="B41" s="2">
-        <v>-81.670599999999993</v>
+        <v>-82.683899999999994</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" s="2">
-        <v>29.702999999999999</v>
+        <v>29.651599999999998</v>
       </c>
       <c r="B42" s="2">
-        <v>-82.383200000000002</v>
+        <v>-82.324799999999996</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A43" s="2">
-        <v>26.154199999999999</v>
+        <v>26.2712</v>
       </c>
       <c r="B43" s="2">
-        <v>-80.299800000000005</v>
+        <v>-80.270600000000002</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A44" s="2">
-        <v>26.663</v>
+        <v>28.612200000000001</v>
       </c>
       <c r="B44" s="2">
-        <v>-81.953500000000005</v>
+        <v>-81.439400000000006</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A45" s="2">
-        <v>28.8005</v>
+        <v>27.447399999999998</v>
       </c>
       <c r="B45" s="2">
-        <v>-82.538700000000006</v>
+        <v>-82.609899999999996</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A46" s="2">
-        <v>29.728999999999999</v>
+        <v>25.7605</v>
       </c>
       <c r="B46" s="2">
-        <v>-85.032200000000003</v>
+        <v>-80.293899999999994</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A47" s="2">
-        <v>30.080200000000001</v>
+        <v>30.401700000000002</v>
       </c>
       <c r="B47" s="2">
-        <v>-81.709299999999999</v>
+        <v>-86.862200000000001</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A48" s="2">
-        <v>29.884899999999998</v>
+        <v>28.660799999999998</v>
       </c>
       <c r="B48" s="2">
-        <v>-81.3155</v>
+        <v>-81.365600000000001</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A49" s="2">
-        <v>27.9726</v>
+        <v>26.128499999999999</v>
       </c>
       <c r="B49" s="2">
-        <v>-82.467600000000004</v>
+        <v>-80.248699999999999</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.4">
       <c r="A50" s="2">
-        <v>28.121600000000001</v>
+        <v>30.521000000000001</v>
       </c>
       <c r="B50" s="2">
-        <v>-81.625</v>
+        <v>-86.481899999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A51" s="2">
+        <v>26.703299999999999</v>
+      </c>
+      <c r="B51" s="2">
+        <v>-80.162700000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A52" s="2">
+        <v>28.046800000000001</v>
+      </c>
+      <c r="B52" s="2">
+        <v>-80.588300000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A53" s="2">
+        <v>30.438300000000002</v>
+      </c>
+      <c r="B53" s="2">
+        <v>-86.647499999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A54" s="2">
+        <v>26.193200000000001</v>
+      </c>
+      <c r="B54" s="2">
+        <v>-80.098799999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A55" s="2">
+        <v>27.9209</v>
+      </c>
+      <c r="B55" s="2">
+        <v>-82.320999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A56" s="2">
+        <v>26.190100000000001</v>
+      </c>
+      <c r="B56" s="2">
+        <v>-80.143600000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A57" s="2">
+        <v>27.964200000000002</v>
+      </c>
+      <c r="B57" s="2">
+        <v>-82.447299999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A58" s="2">
+        <v>28.386099999999999</v>
+      </c>
+      <c r="B58" s="2">
+        <v>-81.498099999999994</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A59" s="2">
+        <v>28.5702</v>
+      </c>
+      <c r="B59" s="2">
+        <v>-81.372799999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A60" s="2">
+        <v>29.692499999999999</v>
+      </c>
+      <c r="B60" s="2">
+        <v>-82.348200000000006</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A61" s="2">
+        <v>27.950600000000001</v>
+      </c>
+      <c r="B61" s="2">
+        <v>-82.4572</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A62" s="2">
+        <v>26.0989</v>
+      </c>
+      <c r="B62" s="2">
+        <v>-80.381500000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A63" s="2">
+        <v>28.4161</v>
+      </c>
+      <c r="B63" s="2">
+        <v>-81.307000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A64" s="2">
+        <v>26.2118</v>
+      </c>
+      <c r="B64" s="2">
+        <v>-80.142600000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A65" s="2">
+        <v>30.442699999999999</v>
+      </c>
+      <c r="B65" s="2">
+        <v>-86.652199999999993</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A66" s="2">
+        <v>28.802800000000001</v>
+      </c>
+      <c r="B66" s="2">
+        <v>-81.271100000000004</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2">
+        <v>27.7942</v>
+      </c>
+      <c r="B67" s="2">
+        <v>-82.672899999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A68" s="2">
+        <v>30.1585</v>
+      </c>
+      <c r="B68" s="2">
+        <v>-85.658299999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2">
+        <v>28.054600000000001</v>
+      </c>
+      <c r="B69" s="2">
+        <v>-82.424700000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A70" s="2">
+        <v>26.7117</v>
+      </c>
+      <c r="B70" s="2">
+        <v>-81.863299999999995</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A71" s="2">
+        <v>30.418500000000002</v>
+      </c>
+      <c r="B71" s="2">
+        <v>-86.643199999999993</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A72" s="2">
+        <v>26.1889</v>
+      </c>
+      <c r="B72" s="2">
+        <v>-80.201899999999995</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A73" s="2">
+        <v>29.186299999999999</v>
+      </c>
+      <c r="B73" s="2">
+        <v>-82.131399999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A74" s="2">
+        <v>26.135300000000001</v>
+      </c>
+      <c r="B74" s="2">
+        <v>-80.143100000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A75" s="2">
+        <v>29.212199999999999</v>
+      </c>
+      <c r="B75" s="2">
+        <v>-81.027699999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A76" s="2">
+        <v>27.984000000000002</v>
+      </c>
+      <c r="B76" s="2">
+        <v>-82.792500000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2">
+        <v>28.898099999999999</v>
+      </c>
+      <c r="B77" s="2">
+        <v>-81.9298</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A78" s="2">
+        <v>26.075500000000002</v>
+      </c>
+      <c r="B78" s="2">
+        <v>-80.236800000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A79" s="2">
+        <v>30.331199999999999</v>
+      </c>
+      <c r="B79" s="2">
+        <v>-81.655500000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A80" s="2">
+        <v>29.124199999999998</v>
+      </c>
+      <c r="B80" s="2">
+        <v>-82.009699999999995</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A81" s="2">
+        <v>28.606400000000001</v>
+      </c>
+      <c r="B81" s="2">
+        <v>-81.383399999999995</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A82" s="2">
+        <v>28.5749</v>
+      </c>
+      <c r="B82" s="2">
+        <v>-81.398499999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A83" s="2">
+        <v>29.759399999999999</v>
+      </c>
+      <c r="B83" s="2">
+        <v>-84.870900000000006</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A84" s="2">
+        <v>26.610499999999998</v>
+      </c>
+      <c r="B84" s="2">
+        <v>-81.870599999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2">
+        <v>30.333100000000002</v>
+      </c>
+      <c r="B85" s="2">
+        <v>-81.655699999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A86" s="2">
+        <v>27.9466</v>
+      </c>
+      <c r="B86" s="2">
+        <v>-82.458100000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A87" s="2">
+        <v>30.2685</v>
+      </c>
+      <c r="B87" s="2">
+        <v>-81.530600000000007</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A88" s="2">
+        <v>30.338100000000001</v>
+      </c>
+      <c r="B88" s="2">
+        <v>-81.419799999999995</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A89" s="2">
+        <v>30.058299999999999</v>
+      </c>
+      <c r="B89" s="2">
+        <v>-81.717200000000005</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A90" s="2">
+        <v>28.782699999999998</v>
+      </c>
+      <c r="B90" s="2">
+        <v>-81.292599999999993</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A91" s="2">
+        <v>27.908899999999999</v>
+      </c>
+      <c r="B91" s="2">
+        <v>-82.323599999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A92" s="2">
+        <v>30.280899999999999</v>
+      </c>
+      <c r="B92" s="2">
+        <v>-81.396500000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A93" s="2">
+        <v>28.8292</v>
+      </c>
+      <c r="B93" s="2">
+        <v>-82.057199999999995</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A94" s="2">
+        <v>27.910499999999999</v>
+      </c>
+      <c r="B94" s="2">
+        <v>-82.316599999999994</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A95" s="2">
+        <v>28.051500000000001</v>
+      </c>
+      <c r="B95" s="2">
+        <v>-82.525899999999993</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A96" s="2">
+        <v>30.257400000000001</v>
+      </c>
+      <c r="B96" s="2">
+        <v>-81.500399999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A97" s="2">
+        <v>30.314800000000002</v>
+      </c>
+      <c r="B97" s="2">
+        <v>-81.686199999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A98" s="2">
+        <v>27.334099999999999</v>
+      </c>
+      <c r="B98" s="2">
+        <v>-82.538700000000006</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A99" s="2">
+        <v>28.847100000000001</v>
+      </c>
+      <c r="B99" s="2">
+        <v>-81.648499999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A100" s="2">
+        <v>28.815899999999999</v>
+      </c>
+      <c r="B100" s="2">
+        <v>-81.901700000000005</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A101" s="2">
+        <v>30.289300000000001</v>
+      </c>
+      <c r="B101" s="2">
+        <v>-81.393500000000003</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A102" s="2">
+        <v>28.801400000000001</v>
+      </c>
+      <c r="B102" s="2">
+        <v>-81.272099999999995</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A103" s="2">
+        <v>29.6325</v>
+      </c>
+      <c r="B103" s="2">
+        <v>-82.343100000000007</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A104" s="2">
+        <v>28.562200000000001</v>
+      </c>
+      <c r="B104" s="2">
+        <v>-81.352500000000006</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A105" s="2">
+        <v>27.901700000000002</v>
+      </c>
+      <c r="B105" s="2">
+        <v>-82.301400000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A106" s="2">
+        <v>29.6113</v>
+      </c>
+      <c r="B106" s="2">
+        <v>-82.374899999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A107" s="2">
+        <v>30.220099999999999</v>
+      </c>
+      <c r="B107" s="2">
+        <v>-81.605900000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A108" s="2">
+        <v>28.601700000000001</v>
+      </c>
+      <c r="B108" s="2">
+        <v>-81.307100000000005</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A109" s="2">
+        <v>28.913799999999998</v>
+      </c>
+      <c r="B109" s="2">
+        <v>-81.304599999999994</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A110" s="2">
+        <v>30.287600000000001</v>
+      </c>
+      <c r="B110" s="2">
+        <v>-81.392200000000003</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A111" s="2">
+        <v>30.198399999999999</v>
+      </c>
+      <c r="B111" s="2">
+        <v>-81.715699999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A112" s="2">
+        <v>29.650600000000001</v>
+      </c>
+      <c r="B112" s="2">
+        <v>-82.326899999999995</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A113" s="2">
+        <v>28.8278</v>
+      </c>
+      <c r="B113" s="2">
+        <v>-82.320099999999996</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A114" s="2">
+        <v>30.088899999999999</v>
+      </c>
+      <c r="B114" s="2">
+        <v>-81.706800000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A115" s="2">
+        <v>27.7925</v>
+      </c>
+      <c r="B115" s="2">
+        <v>-82.632800000000003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A116" s="2">
+        <v>30.2805</v>
+      </c>
+      <c r="B116" s="2">
+        <v>-81.395899999999997</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A117" s="2">
+        <v>28.5991</v>
+      </c>
+      <c r="B117" s="2">
+        <v>-81.249399999999994</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A118" s="2">
+        <v>27.463899999999999</v>
+      </c>
+      <c r="B118" s="2">
+        <v>-82.576700000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A119" s="2">
+        <v>29.6173</v>
+      </c>
+      <c r="B119" s="2">
+        <v>-82.371399999999994</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A120" s="2">
+        <v>29.208227999999998</v>
+      </c>
+      <c r="B120" s="2">
+        <v>-82.096145000000007</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A121" s="2">
+        <v>30.442416999999999</v>
+      </c>
+      <c r="B121" s="2">
+        <v>-84.292811</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A122" s="2">
+        <v>30.284976</v>
+      </c>
+      <c r="B122" s="2">
+        <v>-81.393683999999993</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A123" s="2">
+        <v>28.546011</v>
+      </c>
+      <c r="B123" s="2">
+        <v>-81.373355000000004</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A124" s="2">
+        <v>29.637729</v>
+      </c>
+      <c r="B124" s="2">
+        <v>-82.347209000000007</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A125" s="2">
+        <v>30.713502999999999</v>
+      </c>
+      <c r="B125" s="2">
+        <v>-86.583315999999996</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A126" s="2">
+        <v>26.621811000000001</v>
+      </c>
+      <c r="B126" s="2">
+        <v>-81.840063999999998</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A127" s="2">
+        <v>30.358307</v>
+      </c>
+      <c r="B127" s="2">
+        <v>-87.308935000000005</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A128" s="2">
+        <v>27.174624000000001</v>
+      </c>
+      <c r="B128" s="2">
+        <v>-80.256507999999997</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A129" s="2">
+        <v>29.406542000000002</v>
+      </c>
+      <c r="B129" s="2">
+        <v>-82.177745999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A130" s="2">
+        <v>28.545901000000001</v>
+      </c>
+      <c r="B130" s="2">
+        <v>-81.384709000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A131" s="2">
+        <v>29.648675999999998</v>
+      </c>
+      <c r="B131" s="2">
+        <v>-82.341123999999994</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A132" s="2">
+        <v>30.425139000000001</v>
+      </c>
+      <c r="B132" s="2">
+        <v>-86.646528000000004</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A133" s="2">
+        <v>26.608322999999999</v>
+      </c>
+      <c r="B133" s="2">
+        <v>-81.843539000000007</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A134" s="2">
+        <v>26.114775999999999</v>
+      </c>
+      <c r="B134" s="2">
+        <v>-80.145037000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A135" s="2">
+        <v>27.763636000000002</v>
+      </c>
+      <c r="B135" s="2">
+        <v>-82.635834000000003</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A136" s="2">
+        <v>27.3298308</v>
+      </c>
+      <c r="B136" s="2">
+        <v>-82.539264000000003</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A137" s="2">
+        <v>28.811447000000001</v>
+      </c>
+      <c r="B137" s="2">
+        <v>-81.358732000000003</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A138" s="2">
+        <v>28.967229700000001</v>
+      </c>
+      <c r="B138" s="2">
+        <v>-81.899494000000004</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A139" s="2">
+        <v>27.7700076</v>
+      </c>
+      <c r="B139" s="2">
+        <v>-82.636054000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A140" s="2">
+        <v>27.809994499999998</v>
+      </c>
+      <c r="B140" s="2">
+        <v>-82.679265999999998</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A141" s="2">
+        <v>26.011201400000001</v>
+      </c>
+      <c r="B141" s="2">
+        <v>-80.14949</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A142" s="2">
+        <v>28.538335499999999</v>
+      </c>
+      <c r="B142" s="2">
+        <v>-81.379236000000006</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A143" s="2">
+        <v>30.402974</v>
+      </c>
+      <c r="B143" s="2">
+        <v>-86.861345</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A144" s="2">
+        <v>26.635231000000001</v>
+      </c>
+      <c r="B144" s="2">
+        <v>-80.096435999999997</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A145" s="2">
+        <v>26.197969799999999</v>
+      </c>
+      <c r="B145" s="2">
+        <v>-80.131974999999997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A146" s="2">
+        <v>26.268691</v>
+      </c>
+      <c r="B146" s="2">
+        <v>-80.088561999999996</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A147" s="2">
+        <v>26.343582000000001</v>
+      </c>
+      <c r="B147" s="2">
+        <v>-80.102514999999997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A148" s="2">
+        <v>26.274398000000001</v>
+      </c>
+      <c r="B148" s="2">
+        <v>-80.134556000000003</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A149" s="2">
+        <v>25.881509000000001</v>
+      </c>
+      <c r="B149" s="2">
+        <v>-80.319569999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A150" s="2">
+        <v>26.121162000000002</v>
+      </c>
+      <c r="B150" s="2">
+        <v>-80.140332999999998</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A151" s="2">
+        <v>26.246638000000001</v>
+      </c>
+      <c r="B151" s="2">
+        <v>-80.123741999999993</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A152" s="2">
+        <v>25.978119</v>
+      </c>
+      <c r="B152" s="2">
+        <v>-80.219268</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A153" s="2">
+        <v>27.950575000000001</v>
+      </c>
+      <c r="B153" s="2">
+        <v>-82.457177000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A154" s="2">
+        <v>25.911563000000001</v>
+      </c>
+      <c r="B154" s="2">
+        <v>-80.309269999999998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A155" s="2">
+        <v>28.034461</v>
+      </c>
+      <c r="B155" s="2">
+        <v>-81.949703999999997</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A156" s="2">
+        <v>26.082131</v>
+      </c>
+      <c r="B156" s="2">
+        <v>-80.360647</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A157" s="2">
+        <v>27.947759000000001</v>
+      </c>
+      <c r="B157" s="2">
+        <v>-82.458444</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A158" s="2">
+        <v>26.126325999999999</v>
+      </c>
+      <c r="B158" s="2">
+        <v>-80.261881000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A159" s="2">
+        <v>26.212982</v>
+      </c>
+      <c r="B159" s="2">
+        <v>-80.150796999999997</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A160" s="2">
+        <v>26.239436000000001</v>
+      </c>
+      <c r="B160" s="2">
+        <v>-80.119825000000006</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A161" s="2">
+        <v>27.950575000000001</v>
+      </c>
+      <c r="B161" s="2">
+        <v>-82.457177000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A162" s="2">
+        <v>26.287716</v>
+      </c>
+      <c r="B162" s="2">
+        <v>-80.202725999999998</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A163" s="2">
+        <v>27.950575000000001</v>
+      </c>
+      <c r="B163" s="2">
+        <v>-82.457177000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A164" s="2">
+        <v>27.882857000000001</v>
+      </c>
+      <c r="B164" s="2">
+        <v>-82.716610000000003</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A165" s="2">
+        <v>28.358433000000002</v>
+      </c>
+      <c r="B165" s="2">
+        <v>-81.421413000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A166" s="2">
+        <v>26.150442999999999</v>
+      </c>
+      <c r="B166" s="2">
+        <v>-80.273773000000006</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A167" s="2">
+        <v>26.378124</v>
+      </c>
+      <c r="B167" s="2">
+        <v>-80.096425999999994</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A168" s="2">
+        <v>27.947759000000001</v>
+      </c>
+      <c r="B168" s="2">
+        <v>-82.458444</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A169" s="2">
+        <v>25.679922000000001</v>
+      </c>
+      <c r="B169" s="2">
+        <v>-80.339206000000004</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A170" s="2">
+        <v>25.790654</v>
+      </c>
+      <c r="B170" s="2">
+        <v>-80.130044999999996</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A171" s="2">
+        <v>26.616696000000001</v>
+      </c>
+      <c r="B171" s="2">
+        <v>-81.872308000000004</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A172" s="2">
+        <v>28.537158000000002</v>
+      </c>
+      <c r="B172" s="2">
+        <v>-81.377370999999997</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A173" s="2">
+        <v>25.997042</v>
+      </c>
+      <c r="B173" s="2">
+        <v>-80.271579000000003</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A174" s="2">
+        <v>28.538335</v>
+      </c>
+      <c r="B174" s="2">
+        <v>-81.377763000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A175" s="2">
+        <v>25.921375999999999</v>
+      </c>
+      <c r="B175" s="2">
+        <v>-80.317122999999995</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A176" s="2">
+        <v>28.545985999999999</v>
+      </c>
+      <c r="B176" s="2">
+        <v>-81.372995000000003</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A177" s="2">
+        <v>28.538335</v>
+      </c>
+      <c r="B177" s="2">
+        <v>-81.377763000000002</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A178" s="2">
+        <v>25.958044000000001</v>
+      </c>
+      <c r="B178" s="2">
+        <v>-80.183164000000005</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A179" s="2">
+        <v>28.539166000000002</v>
+      </c>
+      <c r="B179" s="2">
+        <v>-81.379706999999996</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A180" s="2">
+        <v>25.872205999999998</v>
+      </c>
+      <c r="B180" s="2">
+        <v>-80.318268000000003</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A181" s="2">
+        <v>26.711036</v>
+      </c>
+      <c r="B181" s="2">
+        <v>-81.862005999999994</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A182" s="2">
+        <v>28.049678</v>
+      </c>
+      <c r="B182" s="2">
+        <v>-82.728013000000004</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A183" s="2">
+        <v>27.950575000000001</v>
+      </c>
+      <c r="B183" s="2">
+        <v>-82.457177000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A184" s="2">
+        <v>26.652197000000001</v>
+      </c>
+      <c r="B184" s="2">
+        <v>-81.843031999999994</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A185" s="2">
+        <v>27.950575000000001</v>
+      </c>
+      <c r="B185" s="2">
+        <v>-82.457177000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A186" s="2">
+        <v>25.978119</v>
+      </c>
+      <c r="B186" s="2">
+        <v>-80.219268</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A187" s="2">
+        <v>28.538335</v>
+      </c>
+      <c r="B187" s="2">
+        <v>-81.377763000000002</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A188" s="2">
+        <v>27.952228000000002</v>
+      </c>
+      <c r="B188" s="2">
+        <v>-82.459835999999996</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A189" s="2">
+        <v>25.682628000000001</v>
+      </c>
+      <c r="B189" s="2">
+        <v>-80.316840999999997</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A190" s="2">
+        <v>26.134920000000001</v>
+      </c>
+      <c r="B190" s="2">
+        <v>-80.139634000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A191" s="2">
+        <v>25.687405999999999</v>
+      </c>
+      <c r="B191" s="2">
+        <v>-80.316171999999995</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A192" s="2">
+        <v>27.947759000000001</v>
+      </c>
+      <c r="B192" s="2">
+        <v>-82.458444</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A193" s="2">
+        <v>26.276602</v>
+      </c>
+      <c r="B193" s="2">
+        <v>-80.203373999999997</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A194" s="2">
+        <v>28.538335</v>
+      </c>
+      <c r="B194" s="2">
+        <v>-81.377763000000002</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A195" s="2">
+        <v>26.636737</v>
+      </c>
+      <c r="B195" s="2">
+        <v>-81.872495999999998</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A196" s="2">
+        <v>30.460699999999999</v>
+      </c>
+      <c r="B196" s="2">
+        <v>-87.255799999999994</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A197" s="2">
+        <v>27.755700000000001</v>
+      </c>
+      <c r="B197" s="2">
+        <v>-82.741900000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A198" s="2">
+        <v>25.790700000000001</v>
+      </c>
+      <c r="B198" s="2">
+        <v>-80.13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A199" s="2">
+        <v>29.058800000000002</v>
+      </c>
+      <c r="B199" s="2">
+        <v>-81.0321</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A200" s="2">
+        <v>26.011199999999999</v>
+      </c>
+      <c r="B200" s="2">
+        <v>-80.142799999999994</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A201" s="2">
+        <v>25.78</v>
+      </c>
+      <c r="B201" s="2">
+        <v>-80.180000000000007</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A202" s="2">
+        <v>29.179400000000001</v>
+      </c>
+      <c r="B202" s="2">
+        <v>-82.128</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A203" s="2">
+        <v>26.674199999999999</v>
+      </c>
+      <c r="B203" s="2">
+        <v>-80.058599999999998</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A204" s="2">
+        <v>30.420100000000001</v>
+      </c>
+      <c r="B204" s="2">
+        <v>-86.617000000000004</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A205" s="2">
+        <v>26.122399999999999</v>
+      </c>
+      <c r="B205" s="2">
+        <v>-80.137299999999996</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A206" s="2">
+        <v>30.451499999999999</v>
+      </c>
+      <c r="B206" s="2">
+        <v>-84.268600000000006</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A207" s="2">
+        <v>27.4956</v>
+      </c>
+      <c r="B207" s="2">
+        <v>-81.440700000000007</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A208" s="2">
+        <v>29.74</v>
+      </c>
+      <c r="B208" s="2">
+        <v>-84.870999999999995</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A209" s="2">
+        <v>26.148900000000001</v>
+      </c>
+      <c r="B209" s="2">
+        <v>-80.203999999999994</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A210" s="2">
+        <v>30.331499999999998</v>
+      </c>
+      <c r="B210" s="2">
+        <v>-81.655699999999996</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A211" s="2">
+        <v>26.0078</v>
+      </c>
+      <c r="B211" s="2">
+        <v>-80.296300000000002</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A212" s="2">
+        <v>27.702400000000001</v>
+      </c>
+      <c r="B212" s="2">
+        <v>-82.4024</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A213" s="2">
+        <v>25.988900000000001</v>
+      </c>
+      <c r="B213" s="2">
+        <v>-80.167000000000002</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A214" s="2">
+        <v>26.141999999999999</v>
+      </c>
+      <c r="B214" s="2">
+        <v>-81.794799999999995</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A215" s="2">
+        <v>27.644600000000001</v>
+      </c>
+      <c r="B215" s="2">
+        <v>-81.515799999999999</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A216" s="2">
+        <v>30.422000000000001</v>
+      </c>
+      <c r="B216" s="2">
+        <v>-87.217399999999998</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A217" s="2">
+        <v>27.833300000000001</v>
+      </c>
+      <c r="B217" s="2">
+        <v>-82.724800000000002</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A218" s="2">
+        <v>27.941199999999998</v>
+      </c>
+      <c r="B218" s="2">
+        <v>-81.946100000000001</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A219" s="2">
+        <v>28.042400000000001</v>
+      </c>
+      <c r="B219" s="2">
+        <v>-81.952100000000002</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A220" s="2">
+        <v>30.2029</v>
+      </c>
+      <c r="B220" s="2">
+        <v>-81.640799999999999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A221" s="2">
+        <v>25.745899999999999</v>
+      </c>
+      <c r="B221" s="2">
+        <v>-80.260499999999993</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A222" s="2">
+        <v>26.128599999999999</v>
+      </c>
+      <c r="B222" s="2">
+        <v>-80.141000000000005</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A223" s="2">
+        <v>27.336400000000001</v>
+      </c>
+      <c r="B223" s="2">
+        <v>-82.530699999999996</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A224" s="2">
+        <v>27.447800000000001</v>
+      </c>
+      <c r="B224" s="2">
+        <v>-80.325599999999994</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A225" s="2">
+        <v>30.734999999999999</v>
+      </c>
+      <c r="B225" s="2">
+        <v>-86.602999999999994</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A226" s="2">
+        <v>30.2944</v>
+      </c>
+      <c r="B226" s="2">
+        <v>-82.984200000000001</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A227" s="2">
+        <v>28.080500000000001</v>
+      </c>
+      <c r="B227" s="2">
+        <v>-80.608099999999993</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A228" s="2">
+        <v>27.947500000000002</v>
+      </c>
+      <c r="B228" s="2">
+        <v>-82.458399999999997</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A229" s="2">
+        <v>28.078099999999999</v>
+      </c>
+      <c r="B229" s="2">
+        <v>-82.758700000000005</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A230" s="2">
+        <v>28.2742</v>
+      </c>
+      <c r="B230" s="2">
+        <v>-81.467500000000001</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A231" s="2">
+        <v>29.651599999999998</v>
+      </c>
+      <c r="B231" s="2">
+        <v>-82.324799999999996</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A232" s="2">
+        <v>26.507400000000001</v>
+      </c>
+      <c r="B232" s="2">
+        <v>-80.075900000000004</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A233" s="2">
+        <v>26.2044</v>
+      </c>
+      <c r="B233" s="2">
+        <v>-80.144099999999995</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A234" s="2">
+        <v>28.811900000000001</v>
+      </c>
+      <c r="B234" s="2">
+        <v>-81.269499999999994</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A235" s="2">
+        <v>26.919499999999999</v>
+      </c>
+      <c r="B235" s="2">
+        <v>-80.112300000000005</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A236" s="2">
+        <v>30.626000000000001</v>
+      </c>
+      <c r="B236" s="2">
+        <v>-87.052300000000002</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A237" s="2">
+        <v>28.858799999999999</v>
+      </c>
+      <c r="B237" s="2">
+        <v>-82.328999999999994</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A238" s="2">
+        <v>27.485600000000002</v>
+      </c>
+      <c r="B238" s="2">
+        <v>-82.580399999999997</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A239" s="2">
+        <v>27.5336</v>
+      </c>
+      <c r="B239" s="2">
+        <v>-82.552700000000002</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A240" s="2">
+        <v>27.291599999999999</v>
+      </c>
+      <c r="B240" s="2">
+        <v>-82.472200000000001</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A241" s="2">
+        <v>26.643599999999999</v>
+      </c>
+      <c r="B241" s="2">
+        <v>-81.8733</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A242" s="2">
+        <v>26.3184</v>
+      </c>
+      <c r="B242" s="2">
+        <v>-80.099800000000002</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A243" s="2">
+        <v>28.791699999999999</v>
+      </c>
+      <c r="B243" s="2">
+        <v>-81.368700000000004</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A244" s="2">
+        <v>27.539300000000001</v>
+      </c>
+      <c r="B244" s="2">
+        <v>-81.374799999999993</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A245" s="2">
+        <v>30.4955</v>
+      </c>
+      <c r="B245" s="2">
+        <v>-84.280699999999996</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A246" s="2">
+        <v>28.0778</v>
+      </c>
+      <c r="B246" s="2">
+        <v>-80.602999999999994</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A247" s="2">
+        <v>29.646599999999999</v>
+      </c>
+      <c r="B247" s="2">
+        <v>-82.322599999999994</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A248" s="2">
+        <v>28.900500000000001</v>
+      </c>
+      <c r="B248" s="2">
+        <v>-82.4435</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A249" s="2">
+        <v>28.536899999999999</v>
+      </c>
+      <c r="B249" s="2">
+        <v>-81.385099999999994</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A250" s="2">
+        <v>27.323599999999999</v>
+      </c>
+      <c r="B250" s="2">
+        <v>-82.3215</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A251" s="2">
+        <v>30.453900000000001</v>
+      </c>
+      <c r="B251" s="2">
+        <v>-82.931799999999996</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A252" s="2">
+        <v>29.7685</v>
+      </c>
+      <c r="B252" s="2">
+        <v>-82.588899999999995</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A253" s="2">
+        <v>27.2911</v>
+      </c>
+      <c r="B253" s="2">
+        <v>-82.4666</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A254" s="2">
+        <v>29.166899999999998</v>
+      </c>
+      <c r="B254" s="2">
+        <v>-81.849500000000006</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A255" s="2">
+        <v>26.099900000000002</v>
+      </c>
+      <c r="B255" s="2">
+        <v>-80.263999999999996</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A256" s="2">
+        <v>28.54</v>
+      </c>
+      <c r="B256" s="2">
+        <v>-81.378900000000002</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A257" s="2">
+        <v>30.3322</v>
+      </c>
+      <c r="B257" s="2">
+        <v>-81.655699999999996</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A258" s="2">
+        <v>27.4467</v>
+      </c>
+      <c r="B258" s="2">
+        <v>-82.359499999999997</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A259" s="2">
+        <v>30.513400000000001</v>
+      </c>
+      <c r="B259" s="2">
+        <v>-87.218199999999996</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A260" s="2">
+        <v>26.128900000000002</v>
+      </c>
+      <c r="B260" s="2">
+        <v>-80.142200000000003</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A261" s="2">
+        <v>29.233599999999999</v>
+      </c>
+      <c r="B261" s="2">
+        <v>-81.068299999999994</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A262" s="2">
+        <v>26.925799999999999</v>
+      </c>
+      <c r="B262" s="2">
+        <v>-80.102800000000002</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A263" s="2">
+        <v>29.934000000000001</v>
+      </c>
+      <c r="B263" s="2">
+        <v>-81.349000000000004</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A264" s="2">
+        <v>30.678699999999999</v>
+      </c>
+      <c r="B264" s="2">
+        <v>-86.165300000000002</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A265" s="2">
+        <v>26.354500000000002</v>
+      </c>
+      <c r="B265" s="2">
+        <v>-81.790700000000001</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A266" s="2">
+        <v>27.273</v>
+      </c>
+      <c r="B266" s="2">
+        <v>-80.3553</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A267" s="2">
+        <v>26.708500000000001</v>
+      </c>
+      <c r="B267" s="2">
+        <v>-80.055000000000007</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A268" s="2">
+        <v>26.022200000000002</v>
+      </c>
+      <c r="B268" s="2">
+        <v>-80.137600000000006</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A269" s="2">
+        <v>27.3721</v>
+      </c>
+      <c r="B269" s="2">
+        <v>-80.372500000000002</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A270" s="2">
+        <v>28.600100000000001</v>
+      </c>
+      <c r="B270" s="2">
+        <v>-81.196799999999996</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A271" s="2">
+        <v>27.527799999999999</v>
+      </c>
+      <c r="B271" s="2">
+        <v>-82.575699999999998</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A272" s="2">
+        <v>28.4773</v>
+      </c>
+      <c r="B272" s="2">
+        <v>-80.685000000000002</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A273" s="2">
+        <v>27.698468999999999</v>
+      </c>
+      <c r="B273" s="2">
+        <v>-80.385794000000004</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A274" s="2">
+        <v>28.435223000000001</v>
+      </c>
+      <c r="B274" s="2">
+        <v>-81.570276000000007</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A275" s="2">
+        <v>26.745826999999998</v>
+      </c>
+      <c r="B275" s="2">
+        <v>-81.899142999999995</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A276" s="2">
+        <v>26.71744</v>
+      </c>
+      <c r="B276" s="2">
+        <v>-81.870903999999996</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A277" s="2">
+        <v>26.570941999999999</v>
+      </c>
+      <c r="B277" s="2">
+        <v>-80.085345000000004</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A278" s="2">
+        <v>26.037922999999999</v>
+      </c>
+      <c r="B278" s="2">
+        <v>-80.135063000000002</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A279" s="2">
+        <v>30.200754</v>
+      </c>
+      <c r="B279" s="2">
+        <v>-85.760226000000003</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A280" s="2">
+        <v>29.202265000000001</v>
+      </c>
+      <c r="B280" s="2">
+        <v>-81.094881000000001</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A281" s="2">
+        <v>26.322634999999998</v>
+      </c>
+      <c r="B281" s="2">
+        <v>-81.790239999999997</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A282" s="2">
+        <v>26.627739999999999</v>
+      </c>
+      <c r="B282" s="2">
+        <v>-81.938912999999999</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A283" s="2">
+        <v>30.299465999999999</v>
+      </c>
+      <c r="B283" s="2">
+        <v>-82.993433999999993</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A284" s="2">
+        <v>27.45091</v>
+      </c>
+      <c r="B284" s="2">
+        <v>-80.466892999999999</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A285" s="2">
+        <v>27.566538999999999</v>
+      </c>
+      <c r="B285" s="2">
+        <v>-80.389657999999997</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A286" s="2">
+        <v>26.214452000000001</v>
+      </c>
+      <c r="B286" s="2">
+        <v>-81.768004000000005</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A287" s="2">
+        <v>29.326612999999998</v>
+      </c>
+      <c r="B287" s="2">
+        <v>-82.228464000000002</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A288" s="2">
+        <v>27.186591</v>
+      </c>
+      <c r="B288" s="2">
+        <v>-82.486937999999995</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A289" s="2">
+        <v>28.32658</v>
+      </c>
+      <c r="B289" s="2">
+        <v>-81.470184000000003</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A290" s="2">
+        <v>25.631011000000001</v>
+      </c>
+      <c r="B290" s="2">
+        <v>-80.434569999999994</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A291" s="2">
+        <v>26.610536</v>
+      </c>
+      <c r="B291" s="2">
+        <v>-81.871948000000003</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A292" s="2">
+        <v>26.650212</v>
+      </c>
+      <c r="B292" s="2">
+        <v>-82.028198000000003</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A293" s="2">
+        <v>30.000903999999998</v>
+      </c>
+      <c r="B293" s="2">
+        <v>-82.415160999999998</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A294" s="2">
+        <v>25.986125999999999</v>
+      </c>
+      <c r="B294" s="2">
+        <v>-80.140991</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A295" s="2">
+        <v>26.994627000000001</v>
+      </c>
+      <c r="B295" s="2">
+        <v>-82.253722999999994</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A296" s="2">
+        <v>27.341398999999999</v>
+      </c>
+      <c r="B296" s="2">
+        <v>-82.438964999999996</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="15" x14ac:dyDescent="0.4">
+      <c r="A297" s="2">
+        <v>28.352058</v>
+      </c>
+      <c r="B297" s="2">
+        <v>-81.366271999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>